<commit_message>
create inflation driver added
</commit_message>
<xml_diff>
--- a/Input/Correlation/correlationmatrix.xlsx
+++ b/Input/Correlation/correlationmatrix.xlsx
@@ -5,24 +5,32 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JQ228YH\Documents\CVA Tool Python\CVA-Tool\Risk Driver Simulation\Input\Correlation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JQ228YH\Documents\CVA Tool Python\CVA-Tool\Input\Correlation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F2A6DE-5833-4B1A-88BA-06336381F63A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B2B643-081C-4A39-B3D4-C473ECE79C94}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-6465" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>EUR</t>
   </si>
@@ -31,6 +39,9 @@
   </si>
   <si>
     <t>EURUSD</t>
+  </si>
+  <si>
+    <t>EURINFL</t>
   </si>
 </sst>
 </file>
@@ -410,7 +421,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -425,6 +436,9 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -439,7 +453,10 @@
       <c r="D2" s="1">
         <v>3.3731999999999998E-2</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="1">
+        <f>B5</f>
+        <v>-0.2</v>
+      </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -457,7 +474,10 @@
       <c r="D3" s="1">
         <v>0.113924</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="1">
+        <f>C5</f>
+        <v>-0.3</v>
+      </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -475,16 +495,30 @@
       <c r="D4" s="1">
         <v>1</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1">
+        <f>D5</f>
+        <v>0.03</v>
+      </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>-0.2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-0.3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>

</xml_diff>

<commit_message>
monte carlo inflation added'
</commit_message>
<xml_diff>
--- a/Input/Correlation/correlationmatrix.xlsx
+++ b/Input/Correlation/correlationmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JQ228YH\Documents\CVA Tool Python\CVA-Tool\Input\Correlation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B2B643-081C-4A39-B3D4-C473ECE79C94}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68AAA7CA-C077-4D5E-BE17-266F1EA1F160}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>EUR</t>
   </si>
@@ -41,7 +41,10 @@
     <t>EURUSD</t>
   </si>
   <si>
-    <t>EURINFL</t>
+    <t>EUR REAL</t>
+  </si>
+  <si>
+    <t>EUR INFL</t>
   </si>
 </sst>
 </file>
@@ -421,7 +424,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -439,6 +442,9 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -457,7 +463,10 @@
         <f>B5</f>
         <v>-0.2</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="1">
+        <f>B6</f>
+        <v>0.3</v>
+      </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
@@ -476,9 +485,12 @@
       </c>
       <c r="E3" s="1">
         <f>C5</f>
-        <v>-0.3</v>
-      </c>
-      <c r="F3" s="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="F3" s="1">
+        <f>C6</f>
+        <v>-0.1</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
@@ -499,7 +511,10 @@
         <f>D5</f>
         <v>0.03</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1">
+        <f>D6</f>
+        <v>0.43</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
@@ -511,7 +526,7 @@
         <v>-0.2</v>
       </c>
       <c r="C5" s="1">
-        <v>-0.3</v>
+        <v>0.95</v>
       </c>
       <c r="D5" s="1">
         <v>0.03</v>
@@ -519,16 +534,32 @@
       <c r="E5" s="1">
         <v>1</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1">
+        <f>E6</f>
+        <v>-0.09</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>-0.1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.43</v>
+      </c>
+      <c r="E6" s="1">
+        <v>-0.09</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>

</xml_diff>

<commit_message>
adding cms spread cap floor
</commit_message>
<xml_diff>
--- a/Input/Correlation/correlationmatrix.xlsx
+++ b/Input/Correlation/correlationmatrix.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JQ228YH\Documents\CVA Tool Python\CVA-Tool\Input\Correlation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68AAA7CA-C077-4D5E-BE17-266F1EA1F160}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0AACE7-EB62-4F83-A117-29D1EB1DAB8A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-6465" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>EUR</t>
   </si>
@@ -38,13 +38,7 @@
     <t>USD</t>
   </si>
   <si>
-    <t>EURUSD</t>
-  </si>
-  <si>
-    <t>EUR REAL</t>
-  </si>
-  <si>
-    <t>EUR INFL</t>
+    <t>USDEUR</t>
   </si>
 </sst>
 </file>
@@ -424,73 +418,61 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
+      <c r="B1" t="str">
+        <f>A2</f>
+        <v>EUR</v>
+      </c>
+      <c r="C1" t="str">
+        <f>A3</f>
+        <v>USD</v>
+      </c>
+      <c r="D1" t="str">
+        <f>A4</f>
+        <v>USDEUR</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>-0.44989699999999999</v>
+        <f>B3</f>
+        <v>0.71960000000000002</v>
       </c>
       <c r="D2" s="1">
-        <v>3.3731999999999998E-2</v>
-      </c>
-      <c r="E2" s="1">
-        <f>B5</f>
-        <v>-0.2</v>
-      </c>
-      <c r="F2" s="1">
-        <f>B6</f>
-        <v>0.3</v>
-      </c>
+        <f>B4</f>
+        <v>-6.4500000000000002E-2</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>-0.44989699999999999</v>
+        <v>0.71960000000000002</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>0.113924</v>
-      </c>
-      <c r="E3" s="1">
-        <f>C5</f>
-        <v>0.95</v>
-      </c>
-      <c r="F3" s="1">
-        <f>C6</f>
-        <v>-0.1</v>
-      </c>
+        <f>C4</f>
+        <v>7.6300000000000007E-2</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
@@ -499,67 +481,34 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>3.3731999999999998E-2</v>
+        <v>-6.4500000000000002E-2</v>
       </c>
       <c r="C4" s="1">
-        <v>0.113924</v>
+        <v>7.6300000000000007E-2</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
       </c>
-      <c r="E4" s="1">
-        <f>D5</f>
-        <v>0.03</v>
-      </c>
-      <c r="F4" s="1">
-        <f>D6</f>
-        <v>0.43</v>
-      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1">
-        <v>-0.2</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1">
-        <f>E6</f>
-        <v>-0.09</v>
-      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="C6" s="1">
-        <v>-0.1</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.43</v>
-      </c>
-      <c r="E6" s="1">
-        <v>-0.09</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>

</xml_diff>